<commit_message>
Update auf Spring Boot 2.0.1
</commit_message>
<xml_diff>
--- a/src/test/resources/AWK.xlsx
+++ b/src/test/resources/AWK.xlsx
@@ -807,7 +807,7 @@
       <sheetData sheetId="0">
         <row r="4">
           <cell r="H4">
-            <v>43131</v>
+            <v>43132</v>
           </cell>
           <cell r="I4">
             <v>43101</v>
@@ -27684,7 +27684,7 @@
   <dimension ref="A1:NT55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7:N55"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31100,7 +31100,7 @@
       </c>
       <c r="H4" s="21">
         <f ca="1">TODAY()</f>
-        <v>43131</v>
+        <v>43132</v>
       </c>
       <c r="I4" s="22">
         <v>43101</v>

</xml_diff>